<commit_message>
DOCS: updating the README with database Models and structure
</commit_message>
<xml_diff>
--- a/static/assets/README/Insight_Database_Design.xlsx
+++ b/static/assets/README/Insight_Database_Design.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mazenalali/Developmentproject/Code_Institute_Projects/PP_4_Django/Insights/static/assets/README/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D09FB210-967A-C749-AD5D-31D36CB5162B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33C00305-0AE8-2B4A-80D2-CADD6348C846}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="2360" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{8258824B-1842-D643-B381-CA45A86C2B31}"/>
+    <workbookView xWindow="380" yWindow="920" windowWidth="25620" windowHeight="17440" activeTab="1" xr2:uid="{8258824B-1842-D643-B381-CA45A86C2B31}"/>
   </bookViews>
   <sheets>
     <sheet name="Authro" sheetId="1" r:id="rId1"/>
-    <sheet name="Category" sheetId="2" r:id="rId2"/>
-    <sheet name="Book" sheetId="3" r:id="rId3"/>
-    <sheet name="Likes" sheetId="4" r:id="rId4"/>
-    <sheet name="Rating" sheetId="5" r:id="rId5"/>
-    <sheet name="User" sheetId="6" r:id="rId6"/>
+    <sheet name="Reveiw" sheetId="7" r:id="rId2"/>
+    <sheet name="Category" sheetId="2" r:id="rId3"/>
+    <sheet name="Book" sheetId="3" r:id="rId4"/>
+    <sheet name="Likes" sheetId="4" r:id="rId5"/>
+    <sheet name="Rating" sheetId="5" r:id="rId6"/>
+    <sheet name="User" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="54">
   <si>
     <t>Author</t>
   </si>
@@ -85,9 +86,6 @@
     <t>approved</t>
   </si>
   <si>
-    <t>Integer</t>
-  </si>
-  <si>
     <t>DateTime</t>
   </si>
   <si>
@@ -101,6 +99,111 @@
   </si>
   <si>
     <t>BooleanField</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Attrib.</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>category_name</t>
+  </si>
+  <si>
+    <t>category_description</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>author_id</t>
+  </si>
+  <si>
+    <t>book_category</t>
+  </si>
+  <si>
+    <t>cover_img</t>
+  </si>
+  <si>
+    <t>short_description</t>
+  </si>
+  <si>
+    <t>SlugField</t>
+  </si>
+  <si>
+    <t>Boolean</t>
+  </si>
+  <si>
+    <t>Likes</t>
+  </si>
+  <si>
+    <t>created_on</t>
+  </si>
+  <si>
+    <t>liked_book</t>
+  </si>
+  <si>
+    <t>user_Id</t>
+  </si>
+  <si>
+    <t>Liked</t>
+  </si>
+  <si>
+    <t>Rating</t>
+  </si>
+  <si>
+    <t>rated_book</t>
+  </si>
+  <si>
+    <t>user_rated</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>FloatField</t>
+  </si>
+  <si>
+    <t>IntegerField</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Fielname</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>EmailField</t>
+  </si>
+  <si>
+    <t>Fiedlname</t>
+  </si>
+  <si>
+    <t>book_Id</t>
+  </si>
+  <si>
+    <t>insight</t>
+  </si>
+  <si>
+    <t>Review</t>
   </si>
 </sst>
 </file>
@@ -142,8 +245,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -165,12 +271,84 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6B2F8FB8-8205-5C45-BC2D-E23906A94B74}" name="Table2" displayName="Table2" ref="A2:C10" totalsRowShown="0">
-  <autoFilter ref="A2:C10" xr:uid="{6B2F8FB8-8205-5C45-BC2D-E23906A94B74}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{6B2F8FB8-8205-5C45-BC2D-E23906A94B74}" name="Table2" displayName="Table2" ref="A2:C11" totalsRowShown="0">
+  <autoFilter ref="A2:C11" xr:uid="{6B2F8FB8-8205-5C45-BC2D-E23906A94B74}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{0DA8C778-3654-B64F-A0AF-4818A711AED2}" name="Attrib"/>
     <tableColumn id="2" xr3:uid="{3EC8C1DF-D319-6F4C-92EA-7BF969A05148}" name="Fieldname"/>
     <tableColumn id="3" xr3:uid="{6823952A-9305-7946-B31B-802D1DAADF7B}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{6C3EE8A7-B7D2-A944-8C09-D77238FCB327}" name="Table8" displayName="Table8" ref="B2:D8" totalsRowShown="0">
+  <autoFilter ref="B2:D8" xr:uid="{6C3EE8A7-B7D2-A944-8C09-D77238FCB327}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9397DD82-DAED-9B4C-84FB-CC4509FA85EE}" name="Attrib"/>
+    <tableColumn id="2" xr3:uid="{363D4F25-740B-934D-8EB5-8992EAB79901}" name="Fiedlname"/>
+    <tableColumn id="3" xr3:uid="{340451D8-73C3-4A45-B615-90363C723680}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{34FB06DF-625A-A746-BAF5-B0DB67946A82}" name="Table3" displayName="Table3" ref="A2:C5" totalsRowShown="0">
+  <autoFilter ref="A2:C5" xr:uid="{34FB06DF-625A-A746-BAF5-B0DB67946A82}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{48901B4B-C4E5-1348-9BF8-05E700D0D73B}" name="Attrib."/>
+    <tableColumn id="2" xr3:uid="{867D0315-58AE-D742-8003-96A4B9F6F135}" name="Fieldname"/>
+    <tableColumn id="3" xr3:uid="{D8E15970-7D72-8642-97BA-7209888B4CDC}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B28BFE30-21C6-E94C-9D07-B5CC5EE2BAF6}" name="Table4" displayName="Table4" ref="A2:C11" totalsRowShown="0">
+  <autoFilter ref="A2:C11" xr:uid="{B28BFE30-21C6-E94C-9D07-B5CC5EE2BAF6}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2E9A6E96-8B59-3F49-9CD6-0554BAB81480}" name="Attrib."/>
+    <tableColumn id="2" xr3:uid="{F0470F26-112B-C847-9598-A1D0EF8674F5}" name="Fieldname"/>
+    <tableColumn id="3" xr3:uid="{9166E6D0-B03D-1747-A75E-1A58C5BFFAB9}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{FE0F6CEB-BF46-084B-AC26-43F0C4B2194A}" name="Table5" displayName="Table5" ref="A2:C7" totalsRowShown="0">
+  <autoFilter ref="A2:C7" xr:uid="{FE0F6CEB-BF46-084B-AC26-43F0C4B2194A}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9BAFC708-6D73-4D4B-A56F-C204EC83A157}" name="Attrib."/>
+    <tableColumn id="2" xr3:uid="{3A28C0C0-770E-1A4F-8CBE-763ED68AB458}" name="Fieldname"/>
+    <tableColumn id="3" xr3:uid="{E7924BC2-50AF-1F41-A286-91EBECB408BC}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{3CDB6FB8-4F79-2B48-854B-316D1983C121}" name="Table6" displayName="Table6" ref="A2:C6" totalsRowShown="0">
+  <autoFilter ref="A2:C6" xr:uid="{3CDB6FB8-4F79-2B48-854B-316D1983C121}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{65E96263-155A-AA45-9DA2-C0009E5C22D8}" name="Attrib."/>
+    <tableColumn id="2" xr3:uid="{93D0A1C4-3D01-B148-8085-D716225F4638}" name="Fieldname"/>
+    <tableColumn id="3" xr3:uid="{99D6E68A-C263-104D-B2CA-EE6C34D0BF97}" name="Type"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{D59D3A1A-7D64-C543-90B7-8D3E8C662045}" name="Table7" displayName="Table7" ref="A2:C6" totalsRowShown="0">
+  <autoFilter ref="A2:C6" xr:uid="{D59D3A1A-7D64-C543-90B7-8D3E8C662045}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{2C69B733-0C90-244E-BCE1-70141F3135DD}" name="Attrib."/>
+    <tableColumn id="2" xr3:uid="{D528AA00-D461-5245-B1C4-7337BBBB98E6}" name="Fielname"/>
+    <tableColumn id="3" xr3:uid="{C9BA1B3D-57CB-F94D-A6AF-BDF85E82BDD0}" name="Type"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -493,10 +671,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E25020D-0E1B-2E4E-8478-6F4090CF8654}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="232" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -507,11 +685,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -532,7 +710,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -543,7 +721,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -554,7 +732,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -562,7 +740,7 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -570,7 +748,7 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -578,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -586,7 +764,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -594,7 +772,15 @@
         <v>13</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -609,63 +795,539 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A16076-B4B6-B84B-92F0-86CC085885B9}">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9B8E343-6511-9942-B90F-9C087750FD79}">
+  <dimension ref="B1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9DB143-8CC9-3941-B4B2-5F3C28BAADC7}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B0D0F-BDE8-B04A-B536-4B2D704699AB}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F4376F-F81D-6A48-BF53-99084913F300}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55932A7A-AE2F-AD4E-BB74-5143D381991A}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="287" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30A16076-B4B6-B84B-92F0-86CC085885B9}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView zoomScale="225" zoomScaleNormal="225" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E9DB143-8CC9-3941-B4B2-5F3C28BAADC7}">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView zoomScale="217" zoomScaleNormal="217" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{099B0D0F-BDE8-B04A-B536-4B2D704699AB}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29F4376F-F81D-6A48-BF53-99084913F300}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScale="230" zoomScaleNormal="230" workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55932A7A-AE2F-AD4E-BB74-5143D381991A}">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>